<commit_message>
Added todo for Haoran
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A72FBC-9B35-48F7-947E-84E1FCB1A0AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE0CD39-9373-4BB8-A51B-35C998CB1CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyBorder="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -643,17 +643,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="16" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Awfull" xfId="6" xr:uid="{A1C64B14-41DC-448D-8E99-AECDB8DBF7EC}"/>
@@ -976,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,11 +1024,11 @@
         <v>19</v>
       </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -1126,11 +1127,11 @@
       </c>
       <c r="C13" s="2"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="26" t="s">
+      <c r="M13" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
     </row>
@@ -1144,7 +1145,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="16"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="28"/>
+      <c r="F14" s="26"/>
       <c r="L14" s="12"/>
       <c r="M14" s="13" t="s">
         <v>73</v>
@@ -1163,11 +1164,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="11"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="27" t="s">
+      <c r="M15" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
@@ -1178,8 +1179,8 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
       <c r="L16" s="18"/>
       <c r="M16" s="17" t="s">
         <v>93</v>
@@ -1196,8 +1197,8 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
       <c r="L17" s="18"/>
       <c r="M17" s="17" t="s">
         <v>94</v>
@@ -1214,8 +1215,8 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
       <c r="L18" s="18"/>
       <c r="M18" s="17" t="s">
         <v>95</v>
@@ -1232,8 +1233,8 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
       <c r="L19" s="18"/>
       <c r="M19" s="17" t="s">
         <v>96</v>
@@ -1253,14 +1254,14 @@
       <c r="E20" s="19"/>
       <c r="F20" s="2"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="27" t="s">
+      <c r="M20" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
@@ -1272,8 +1273,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="2"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
       <c r="L21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
@@ -1285,8 +1286,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="2"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
@@ -1294,8 +1295,8 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
@@ -1303,8 +1304,8 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="21"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
     </row>
@@ -1325,11 +1326,11 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="12"/>
-      <c r="M25" s="27" t="s">
+      <c r="M25" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
     </row>
@@ -1344,7 +1345,7 @@
       <c r="D26" s="19"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="29"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1604,7 +1605,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="16"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="28"/>
+      <c r="G45" s="26"/>
       <c r="M45" s="19" t="s">
         <v>57</v>
       </c>
@@ -1616,11 +1617,11 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="11"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
       <c r="M46" s="17" t="s">
         <v>48</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>123</v>
       </c>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="G47" s="25"/>
       <c r="M47" s="17" t="s">
         <v>126</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>124</v>
       </c>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="G48" s="25"/>
       <c r="M48" s="17" t="s">
         <v>125</v>
       </c>
@@ -1655,19 +1656,26 @@
       <c r="P48" s="18"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="11"/>
-      <c r="M49" s="17" t="s">
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="N49" s="17"/>
+      <c r="N49" s="29"/>
       <c r="O49" s="17"/>
       <c r="P49" s="5"/>
     </row>
@@ -1716,23 +1724,23 @@
       <c r="O53" s="17"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
+      <c r="A54" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="31" t="s">
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="29" t="s">
         <v>42</v>
       </c>
       <c r="N54" s="17"/>
@@ -1978,27 +1986,27 @@
       <c r="N69" s="19"/>
       <c r="O69" s="19"/>
     </row>
-    <row r="70" spans="1:15" s="30" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A70" s="32" t="s">
+    <row r="70" spans="1:15" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A70" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30" t="s">
+    <row r="71" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="28" t="s">
         <v>35</v>
       </c>
       <c r="G71" s="23"/>
       <c r="H71" s="23"/>
       <c r="I71" s="23"/>
       <c r="J71" s="23"/>
-      <c r="M71" s="31" t="s">
+      <c r="M71" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="N71" s="31"/>
-      <c r="O71" s="31"/>
+      <c r="N71" s="29"/>
+      <c r="O71" s="29"/>
     </row>
     <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2065,7 +2073,7 @@
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="33" t="s">
+      <c r="A83" s="31" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aaron's code for the improved save/load system and some remarks and name changes from me.
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE0CD39-9373-4BB8-A51B-35C998CB1CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEDE035-9168-41A2-89A3-A9D7B9B012CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14610" windowHeight="9840" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
   <si>
     <t>Description</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>Disaster</t>
+  </si>
+  <si>
+    <t>Expand 2D engine with buttons, slider, textfields and a file explorer</t>
   </si>
 </sst>
 </file>
@@ -978,7 +981,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1600,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>3</v>
@@ -1717,6 +1720,7 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="11"/>
+      <c r="G53" s="26"/>
       <c r="M53" s="17" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Commented out the UI so you can see what's going on
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEDE035-9168-41A2-89A3-A9D7B9B012CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946DE1D-1F42-4AB2-91A8-29141215BEFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14610" windowHeight="9840" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -981,7 +981,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
God mode added (move the ball using the keyboard)
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946DE1D-1F42-4AB2-91A8-29141215BEFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA5206F-CAD5-4469-9534-DFACF8019635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14610" windowHeight="9840" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyBorder="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -653,6 +653,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -981,7 +982,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1012,7 @@
       <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1027,11 +1028,11 @@
         <v>19</v>
       </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -1130,11 +1131,11 @@
       </c>
       <c r="C13" s="2"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
     </row>
@@ -1167,11 +1168,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="11"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="34" t="s">
+      <c r="M15" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
@@ -1260,11 +1261,11 @@
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="34" t="s">
+      <c r="M20" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
@@ -1329,11 +1330,11 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="12"/>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
     </row>
@@ -1800,9 +1801,9 @@
       <c r="C58"/>
       <c r="E58" s="19"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58"/>
-      <c r="I58"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
       <c r="J58"/>
       <c r="M58" s="17" t="s">
         <v>49</v>
@@ -2032,7 +2033,7 @@
       <c r="H74"/>
       <c r="I74"/>
       <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
+      <c r="K74" s="32"/>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
       <c r="O74" s="8"/>

</xml_diff>

<commit_message>
Added water back in and updated planning
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA1EA2D-C621-4795-958C-A0CAFEE009BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52FBA83-46CE-4C6B-93D0-2E063DD11A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15030" windowHeight="9120" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="138">
   <si>
     <t>Description</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Shooting the ball</t>
   </si>
   <si>
-    <t>Resetting after hitting water</t>
-  </si>
-  <si>
     <t>Editor</t>
   </si>
   <si>
@@ -428,13 +425,28 @@
     <t>MAJOR BUILDS / MILESTONES</t>
   </si>
   <si>
-    <t>René and Aaron</t>
-  </si>
-  <si>
     <t>Disaster</t>
   </si>
   <si>
     <t>Expand 2D engine with buttons, slider, textfields and a file explorer</t>
+  </si>
+  <si>
+    <t>Testing / experiments</t>
+  </si>
+  <si>
+    <t>Second Second order Verlet solver (velocity)</t>
+  </si>
+  <si>
+    <t>Implement a second second order Verlet solver, called velocity Verlet solver</t>
+  </si>
+  <si>
+    <t>René and Ivan</t>
+  </si>
+  <si>
+    <t>Jean, Ivan</t>
+  </si>
+  <si>
+    <t>Resetting after hitting water (non-functional, that's for phase 3)</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyBorder="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -645,9 +657,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -656,6 +665,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -978,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection sqref="A1:T80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1034,7 @@
       <c r="H1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1027,11 +1044,11 @@
         <v>18</v>
       </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -1041,7 +1058,7 @@
     </row>
     <row r="3" spans="1:17" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
@@ -1094,17 +1111,20 @@
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
     </row>
-    <row r="8" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="M8" s="19" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="M8" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
     </row>
     <row r="9" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P9" s="18"/>
@@ -1124,7 +1144,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -1132,16 +1152,16 @@
       </c>
       <c r="C13" s="2"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -1163,23 +1183,26 @@
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="11"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>87</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1189,7 +1212,7 @@
       <c r="I16" s="26"/>
       <c r="L16" s="18"/>
       <c r="M16" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
@@ -1199,6 +1222,9 @@
     <row r="17" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>88</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>3</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1208,7 +1234,7 @@
       <c r="I17" s="26"/>
       <c r="L17" s="18"/>
       <c r="M17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
@@ -1217,7 +1243,10 @@
     </row>
     <row r="18" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>89</v>
+        <v>137</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>3</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1227,7 +1256,7 @@
       <c r="I18" s="26"/>
       <c r="L18" s="18"/>
       <c r="M18" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
@@ -1235,8 +1264,8 @@
       <c r="Q18" s="18"/>
     </row>
     <row r="19" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>90</v>
+      <c r="A19" s="38" t="s">
+        <v>89</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1244,17 +1273,17 @@
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
-      <c r="L19" s="36"/>
+      <c r="L19" s="35"/>
       <c r="M19" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N19" s="29"/>
       <c r="O19" s="29"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
     </row>
     <row r="20" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
@@ -1270,20 +1299,20 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="12"/>
-      <c r="M20" s="35" t="s">
+      <c r="M20" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -1292,7 +1321,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="1"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="26"/>
       <c r="K21" s="1"/>
       <c r="L21" s="12"/>
       <c r="M21" s="13" t="s">
@@ -1311,7 +1340,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -1327,7 +1356,7 @@
       <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="13" t="s">
@@ -1347,140 +1376,140 @@
       <c r="Q25" s="12"/>
     </row>
     <row r="26" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>96</v>
+      <c r="A26" s="42" t="s">
+        <v>95</v>
       </c>
       <c r="D26" s="2"/>
       <c r="L26" s="18"/>
       <c r="M26" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
     </row>
     <row r="27" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>97</v>
+      <c r="A27" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="D27" s="2"/>
       <c r="L27" s="18"/>
       <c r="M27" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
     </row>
     <row r="28" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>100</v>
+      <c r="A28" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="D28" s="2"/>
       <c r="L28" s="18"/>
       <c r="M28" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
     </row>
     <row r="29" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>99</v>
+      <c r="A29" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="D29" s="2"/>
       <c r="L29" s="18"/>
       <c r="M29" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
     </row>
     <row r="30" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>98</v>
+      <c r="A30" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="D30" s="2"/>
       <c r="L30" s="18"/>
       <c r="M30" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>101</v>
+      <c r="A31" s="42" t="s">
+        <v>100</v>
       </c>
       <c r="D31" s="2"/>
       <c r="L31" s="18"/>
       <c r="M31" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="18"/>
     </row>
     <row r="32" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>102</v>
+      <c r="A32" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="D32" s="2"/>
       <c r="L32" s="18"/>
       <c r="M32" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
     </row>
     <row r="33" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>103</v>
+      <c r="A33" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="D33" s="2"/>
       <c r="L33" s="18"/>
       <c r="M33" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
     </row>
     <row r="34" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>104</v>
+      <c r="A34" s="42" t="s">
+        <v>103</v>
       </c>
       <c r="D34" s="2"/>
       <c r="L34" s="18"/>
       <c r="M34" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
     </row>
     <row r="35" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>105</v>
+      <c r="A35" s="42" t="s">
+        <v>104</v>
       </c>
       <c r="D35" s="2"/>
       <c r="L35" s="18"/>
       <c r="M35" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
     </row>
     <row r="36" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>116</v>
+      <c r="A36" s="42" t="s">
+        <v>115</v>
       </c>
       <c r="D36" s="2"/>
       <c r="L36" s="18"/>
       <c r="M36" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>118</v>
+      <c r="A37" s="42" t="s">
+        <v>117</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="3"/>
@@ -1492,13 +1521,13 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="M37" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
     </row>
     <row r="38" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="13" t="s">
@@ -1518,7 +1547,7 @@
       <c r="O38" s="17"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B39" t="s">
@@ -1540,11 +1569,11 @@
       <c r="O39" s="17"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>133</v>
+      <c r="A40" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="16"/>
@@ -1559,7 +1588,7 @@
       <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B41" t="s">
@@ -1576,26 +1605,26 @@
       <c r="P41" s="5"/>
     </row>
     <row r="42" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>120</v>
+      <c r="A42" s="42" t="s">
+        <v>119</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="25"/>
       <c r="M42" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N42" s="17"/>
       <c r="O42" s="17"/>
       <c r="P42" s="18"/>
     </row>
     <row r="43" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>121</v>
+      <c r="A43" s="42" t="s">
+        <v>120</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="25"/>
       <c r="M43" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
@@ -1640,7 +1669,7 @@
       <c r="O46" s="19"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B47" t="s">
@@ -1654,210 +1683,206 @@
       <c r="N47" s="17"/>
       <c r="O47" s="17"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="M48" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="N48" s="34"/>
+      <c r="O48" s="34"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="26"/>
-      <c r="M48" s="17" t="s">
+      <c r="E49" s="2"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="26"/>
+      <c r="M49" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="29" t="s">
-        <v>40</v>
       </c>
       <c r="N49" s="17"/>
       <c r="O49" s="17"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="A50" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="13"/>
-      <c r="M50" s="17" t="s">
-        <v>50</v>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="N50" s="17"/>
       <c r="O50" s="17"/>
     </row>
-    <row r="51" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:16" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="30" t="s">
+    <row r="51" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="M51" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+    </row>
+    <row r="52" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:16" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A53" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="P52" s="36"/>
-    </row>
-    <row r="53" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
+      <c r="P53" s="35"/>
+    </row>
+    <row r="54" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B54" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F53" s="37"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="M53" s="29" t="s">
+      <c r="F54" s="36"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="M54" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="N53" s="29"/>
-      <c r="O53" s="29"/>
-      <c r="P53" s="36"/>
-    </row>
-    <row r="54" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P54" s="36"/>
-    </row>
-    <row r="55" spans="1:16" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A55" s="15" t="s">
+      <c r="N54" s="29"/>
+      <c r="O54" s="29"/>
+      <c r="P54" s="35"/>
+    </row>
+    <row r="55" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P55" s="35"/>
+    </row>
+    <row r="56" spans="1:16" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A56" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="M56" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="11"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
       <c r="M57" s="17" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N57" s="17"/>
       <c r="O57" s="17"/>
     </row>
-    <row r="58" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>124</v>
-      </c>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
       <c r="M58" s="17" t="s">
-        <v>127</v>
+        <v>48</v>
       </c>
       <c r="N58" s="17"/>
       <c r="O58" s="17"/>
     </row>
     <row r="59" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>125</v>
+      <c r="A59" s="42" t="s">
+        <v>123</v>
       </c>
       <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
       <c r="M59" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N59" s="17"/>
       <c r="O59" s="17"/>
     </row>
     <row r="60" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>126</v>
+      <c r="A60" s="42" t="s">
+        <v>124</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="M60" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N60" s="17"/>
       <c r="O60" s="17"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
+    <row r="61" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
       <c r="M61" s="17" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="N61" s="17"/>
       <c r="O61" s="17"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
-        <v>24</v>
+      <c r="A62" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>32</v>
@@ -1872,123 +1897,158 @@
       <c r="J62" s="13"/>
       <c r="K62" s="13"/>
       <c r="M62" s="17" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="A63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="13" t="s">
         <v>32</v>
       </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
       <c r="K63" s="13"/>
       <c r="M63" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N63" s="17"/>
       <c r="O63" s="17"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
       <c r="K64" s="13"/>
-      <c r="M64" s="19"/>
-      <c r="N64" s="19"/>
-      <c r="O64" s="19"/>
-    </row>
-    <row r="65" spans="1:15" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A65" s="30" t="s">
+      <c r="M64" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+    </row>
+    <row r="65" spans="1:15" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="34"/>
+      <c r="O65" s="34"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K66" s="13"/>
+      <c r="M66" s="19"/>
+      <c r="N66" s="19"/>
+      <c r="O66" s="19"/>
+    </row>
+    <row r="67" spans="1:15" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A67" s="30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
+    <row r="68" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="28" t="s">
+      <c r="B68" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="M66" s="29" t="s">
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="M68" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="N66" s="29"/>
-      <c r="O66" s="29"/>
-    </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A68" s="15" t="s">
+      <c r="N68" s="29"/>
+      <c r="O68" s="29"/>
+    </row>
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A70" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="71" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>65</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>66</v>
       </c>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="32"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="8"/>
-    </row>
-    <row r="70" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="32"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+    </row>
+    <row r="72" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="9"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
-        <v>132</v>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="31" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commented out code from Haoran that couldn't compile
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A3784D-4E53-4326-BA79-24DB84D48D38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78DCE4A-5D85-4272-A550-5BF6707282CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Small change to the bot slide and references
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78DCE4A-5D85-4272-A550-5BF6707282CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786E2D7B-78C8-480F-80DE-63C114400C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,6 +522,13 @@
     <font>
       <sz val="16"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,7 +622,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyBorder="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -675,6 +682,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Awfull" xfId="6" xr:uid="{A1C64B14-41DC-448D-8E99-AECDB8DBF7EC}"/>
@@ -998,7 +1010,7 @@
   <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1049,7 @@
       <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1202,7 +1214,7 @@
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="39" t="s">
         <v>87</v>
       </c>
       <c r="B16" s="19" t="s">
@@ -1247,28 +1259,28 @@
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
     </row>
-    <row r="18" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="17" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">

</xml_diff>

<commit_message>
Updated use of 'collision' classes
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0D92B4-A907-4845-A759-B64854BF275D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D983F3-3B29-48BA-90A0-5890548944A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11328" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView xWindow="-108" yWindow="324" windowWidth="30936" windowHeight="16476" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -492,6 +492,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -503,7 +523,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -589,6 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="11" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,6 +629,20 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -933,7 +968,7 @@
   <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,11 +1021,11 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
@@ -1011,10 +1046,10 @@
       <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -1031,8 +1066,8 @@
       <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -1056,6 +1091,8 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -1064,25 +1101,25 @@
       <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="1"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="52" t="s">
+      <c r="L7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
@@ -1093,19 +1130,19 @@
       <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="52" t="s">
+      <c r="L8" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1116,19 +1153,19 @@
       <c r="B9" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="26"/>
       <c r="F9" s="1"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="48" t="s">
+      <c r="L9" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
@@ -1139,19 +1176,19 @@
       <c r="B10" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="61"/>
       <c r="E10" s="26"/>
       <c r="F10" s="1"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
@@ -1162,19 +1199,19 @@
       <c r="B11" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="1"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="53" t="s">
+      <c r="L11" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
@@ -1185,19 +1222,19 @@
       <c r="B12" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="61"/>
       <c r="E12" s="26"/>
       <c r="F12" s="1"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="53" t="s">
+      <c r="L12" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
@@ -1208,26 +1245,26 @@
       <c r="B13" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="61"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="1"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="53" t="s">
+      <c r="L13" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
@@ -1239,8 +1276,8 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="61"/>
       <c r="H15" s="26"/>
       <c r="J15" s="26"/>
     </row>
@@ -1248,8 +1285,8 @@
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
@@ -1257,22 +1294,22 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
@@ -1292,20 +1329,20 @@
       <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="50" t="s">
+      <c r="L18" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1316,8 +1353,8 @@
       <c r="B19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="61"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
@@ -1332,28 +1369,28 @@
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="24"/>
       <c r="L20" s="32"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
     </row>
     <row r="21" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="24"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -1365,14 +1402,14 @@
       <c r="N21" s="34"/>
     </row>
     <row r="22" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="24"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="24"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -1384,28 +1421,32 @@
       <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="63"/>
       <c r="G23" s="24"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="L23" s="51" t="s">
+      <c r="L23" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C24" s="59"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="L24" s="36" t="s">
@@ -1421,6 +1462,8 @@
       <c r="B25" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="63"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="L25" s="36" t="s">
@@ -1436,6 +1479,8 @@
       <c r="B26" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="63"/>
       <c r="F26" s="24"/>
       <c r="L26" s="36" t="s">
         <v>43</v>
@@ -1450,6 +1495,8 @@
       <c r="B27" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="63"/>
       <c r="F27" s="24"/>
       <c r="L27" s="36" t="s">
         <v>45</v>
@@ -1464,6 +1511,8 @@
       <c r="B28" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="63"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="L28" s="36" t="s">
@@ -1479,6 +1528,8 @@
       <c r="B29" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="63"/>
       <c r="G29" s="24"/>
       <c r="L29" s="36" t="s">
         <v>48</v>
@@ -1491,13 +1542,15 @@
       <c r="B30" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C30" s="59"/>
+      <c r="D30" s="63"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="L30" s="48" t="s">
+      <c r="L30" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -1506,6 +1559,8 @@
       <c r="B31" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C31" s="59"/>
+      <c r="D31" s="62"/>
       <c r="G31" s="38"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
@@ -1514,12 +1569,14 @@
       </c>
     </row>
     <row r="32" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="C32" s="59"/>
+      <c r="D32" s="62"/>
       <c r="G32" s="38"/>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
@@ -1528,12 +1585,14 @@
       </c>
     </row>
     <row r="33" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="C33" s="59"/>
+      <c r="D33" s="62"/>
       <c r="G33" s="38"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
@@ -1543,8 +1602,8 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
@@ -1559,8 +1618,8 @@
       <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="61"/>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
@@ -1578,8 +1637,8 @@
       <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="1"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="62"/>
       <c r="E36" s="1"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
@@ -1600,8 +1659,8 @@
       <c r="B37" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="61"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1622,6 +1681,8 @@
       <c r="B38" s="40" t="s">
         <v>72</v>
       </c>
+      <c r="C38" s="56"/>
+      <c r="D38" s="61"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="K38" s="25"/>
@@ -1633,6 +1694,8 @@
     </row>
     <row r="39" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="61"/>
       <c r="K39" s="25"/>
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
@@ -1641,8 +1704,8 @@
       <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="61"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -1660,8 +1723,8 @@
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="1"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
@@ -1682,8 +1745,8 @@
       <c r="B42" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="1"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="45"/>
@@ -1704,8 +1767,8 @@
       <c r="B43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="61"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1720,8 +1783,8 @@
     <row r="44" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="61"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
@@ -1736,8 +1799,8 @@
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="61"/>
       <c r="H45" s="26"/>
       <c r="J45" s="26"/>
       <c r="L45" s="12"/>
@@ -1752,8 +1815,8 @@
       <c r="B46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="61"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="26"/>
@@ -1769,8 +1832,8 @@
     </row>
     <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="61"/>
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
@@ -1787,8 +1850,8 @@
         <v>59</v>
       </c>
       <c r="B48" s="17"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="61"/>
       <c r="H48" s="26"/>
       <c r="J48" s="26"/>
       <c r="K48" s="17"/>
@@ -1804,8 +1867,8 @@
       <c r="B49" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="61"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>

</xml_diff>

<commit_message>
UML diagrams per package
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0D92B4-A907-4845-A759-B64854BF275D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E43149C-542F-43FD-AB4F-C3D340543F2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11328" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView minimized="1" xWindow="53460" yWindow="5580" windowWidth="12870" windowHeight="8610" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -492,6 +492,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -503,7 +523,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -589,6 +609,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="11" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,11 +1021,11 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
@@ -1011,10 +1046,10 @@
       <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -1031,8 +1066,8 @@
       <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -1056,6 +1091,8 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -1064,25 +1101,25 @@
       <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="1"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="52" t="s">
+      <c r="L7" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
@@ -1093,19 +1130,19 @@
       <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="52" t="s">
+      <c r="L8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1116,19 +1153,19 @@
       <c r="B9" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="26"/>
       <c r="F9" s="1"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="48" t="s">
+      <c r="L9" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
@@ -1139,19 +1176,19 @@
       <c r="B10" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="26"/>
       <c r="F10" s="1"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
@@ -1162,19 +1199,19 @@
       <c r="B11" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="1"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="53" t="s">
+      <c r="L11" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
@@ -1185,19 +1222,19 @@
       <c r="B12" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="26"/>
       <c r="F12" s="1"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="53" t="s">
+      <c r="L12" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
@@ -1208,26 +1245,26 @@
       <c r="B13" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="1"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="53" t="s">
+      <c r="L13" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
@@ -1239,8 +1276,8 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="53"/>
       <c r="H15" s="26"/>
       <c r="J15" s="26"/>
     </row>
@@ -1248,8 +1285,8 @@
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
@@ -1257,22 +1294,22 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
@@ -1292,20 +1329,20 @@
       <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="50" t="s">
+      <c r="L18" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1316,8 +1353,8 @@
       <c r="B19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
@@ -1332,28 +1369,28 @@
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="24"/>
       <c r="L20" s="32"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
     </row>
     <row r="21" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="24"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
@@ -1365,14 +1402,14 @@
       <c r="N21" s="34"/>
     </row>
     <row r="22" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="24"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="24"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
@@ -1384,28 +1421,33 @@
       <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C23" s="51"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="L23" s="51" t="s">
+      <c r="L23" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C24" s="51"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="L24" s="36" t="s">
@@ -1421,6 +1463,8 @@
       <c r="B25" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C25" s="51"/>
+      <c r="D25" s="55"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="L25" s="36" t="s">
@@ -1436,6 +1480,9 @@
       <c r="B26" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C26" s="51"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="L26" s="36" t="s">
         <v>43</v>
@@ -1450,6 +1497,8 @@
       <c r="B27" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C27" s="51"/>
+      <c r="D27" s="55"/>
       <c r="F27" s="24"/>
       <c r="L27" s="36" t="s">
         <v>45</v>
@@ -1464,6 +1513,8 @@
       <c r="B28" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C28" s="51"/>
+      <c r="D28" s="55"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="L28" s="36" t="s">
@@ -1479,6 +1530,8 @@
       <c r="B29" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C29" s="51"/>
+      <c r="D29" s="55"/>
       <c r="G29" s="24"/>
       <c r="L29" s="36" t="s">
         <v>48</v>
@@ -1491,13 +1544,15 @@
       <c r="B30" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C30" s="51"/>
+      <c r="D30" s="55"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="L30" s="48" t="s">
+      <c r="L30" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -1506,6 +1561,8 @@
       <c r="B31" s="40" t="s">
         <v>71</v>
       </c>
+      <c r="C31" s="51"/>
+      <c r="D31" s="54"/>
       <c r="G31" s="38"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
@@ -1514,12 +1571,14 @@
       </c>
     </row>
     <row r="32" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="54"/>
       <c r="G32" s="38"/>
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
@@ -1528,12 +1587,14 @@
       </c>
     </row>
     <row r="33" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="54"/>
       <c r="G33" s="38"/>
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
@@ -1543,8 +1604,8 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
@@ -1559,8 +1620,8 @@
       <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
@@ -1578,8 +1639,8 @@
       <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="1"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="1"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
@@ -1600,8 +1661,8 @@
       <c r="B37" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1622,6 +1683,8 @@
       <c r="B38" s="40" t="s">
         <v>72</v>
       </c>
+      <c r="C38" s="48"/>
+      <c r="D38" s="53"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="K38" s="25"/>
@@ -1633,6 +1696,8 @@
     </row>
     <row r="39" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="53"/>
       <c r="K39" s="25"/>
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
@@ -1641,8 +1706,8 @@
       <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -1660,8 +1725,8 @@
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="54"/>
       <c r="E41" s="1"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
@@ -1682,8 +1747,8 @@
       <c r="B42" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="1"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="45"/>
@@ -1704,8 +1769,8 @@
       <c r="B43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -1720,8 +1785,8 @@
     <row r="44" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
@@ -1736,8 +1801,8 @@
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="53"/>
       <c r="H45" s="26"/>
       <c r="J45" s="26"/>
       <c r="L45" s="12"/>
@@ -1752,8 +1817,8 @@
       <c r="B46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="26"/>
@@ -1769,8 +1834,8 @@
     </row>
     <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
@@ -1787,8 +1852,8 @@
         <v>59</v>
       </c>
       <c r="B48" s="17"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="53"/>
       <c r="H48" s="26"/>
       <c r="J48" s="26"/>
       <c r="K48" s="17"/>
@@ -1804,8 +1869,8 @@
       <c r="B49" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="53"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>

</xml_diff>

<commit_message>
The terrain generator now requires a function and there's a start of the function that resets the ball after hitting water
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB30AB9-7481-4E7A-A3EA-CA44648E0CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41CE82B-3D9A-4902-ABF3-A66A61936A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="396" windowWidth="30936" windowHeight="16416" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Reset ball after hitting the water</t>
-  </si>
-  <si>
-    <t>Aaron (with René and Jean helping)</t>
   </si>
   <si>
     <t>Allow the user to select a point along the starting position up to the location where the water was hit using a UI.</t>
@@ -676,6 +673,10 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,10 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1025,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,11 +1076,11 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
@@ -1104,10 +1101,10 @@
       <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
@@ -1124,8 +1121,8 @@
       <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
       <c r="E4" s="46"/>
@@ -1173,11 +1170,11 @@
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="69" t="s">
+      <c r="L7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
@@ -1196,11 +1193,11 @@
       <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="69" t="s">
+      <c r="L8" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1219,16 +1216,16 @@
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="65" t="s">
+      <c r="L9" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="64" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="41" t="s">
@@ -1242,11 +1239,11 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="65" t="s">
+      <c r="L10" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
@@ -1265,11 +1262,11 @@
       <c r="H11" s="1"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="70" t="s">
+      <c r="L11" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
@@ -1288,11 +1285,11 @@
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="70" t="s">
+      <c r="L12" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
@@ -1311,11 +1308,11 @@
       <c r="H13" s="1"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="70" t="s">
+      <c r="L13" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
@@ -1353,9 +1350,9 @@
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
@@ -1397,11 +1394,11 @@
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="67" t="s">
+      <c r="L18" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1493,11 +1490,11 @@
       <c r="G23" s="24"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="L23" s="68" t="s">
+      <c r="L23" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="70"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
@@ -1534,7 +1531,7 @@
       <c r="N25" s="36"/>
     </row>
     <row r="26" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="65" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="40" t="s">
@@ -1568,7 +1565,7 @@
       <c r="N27" s="36"/>
     </row>
     <row r="28" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="65" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="40" t="s">
@@ -1612,11 +1609,11 @@
       <c r="E30" s="55"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="L30" s="65" t="s">
+      <c r="L30" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="65"/>
-      <c r="N30" s="65"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -1936,7 +1933,7 @@
         <v>84</v>
       </c>
       <c r="B49" s="57" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C49" s="49"/>
       <c r="D49" s="53"/>
@@ -1946,7 +1943,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="L49" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M49" s="58"/>
       <c r="N49" s="58"/>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="50" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="57" t="s">
         <v>1</v>
@@ -1967,7 +1964,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="L50" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M50" s="58"/>
       <c r="N50" s="58"/>
@@ -2159,7 +2156,7 @@
       <c r="O63" s="22"/>
     </row>
     <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="72" t="s">
+      <c r="A64" s="64" t="s">
         <v>82</v>
       </c>
       <c r="B64"/>

</xml_diff>

<commit_message>
waterHit now has static methods
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41CE82B-3D9A-4902-ABF3-A66A61936A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19C64D4-821B-46A9-BC17-D72064CB3416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="396" windowWidth="30936" windowHeight="16416" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12876" windowHeight="8616" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="11" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -670,13 +669,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,6 +692,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,23 +1076,23 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
       <c r="K2" s="43"/>
       <c r="L2" s="43"/>
       <c r="M2" s="43"/>
@@ -1101,18 +1101,18 @@
       <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
       <c r="M3" s="43"/>
@@ -1121,16 +1121,16 @@
       <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="43"/>
       <c r="L4" s="43"/>
       <c r="M4" s="43"/>
@@ -1146,9 +1146,9 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="I6" s="26"/>
@@ -1162,19 +1162,19 @@
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
@@ -1185,19 +1185,19 @@
       <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="71" t="s">
+      <c r="L8" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1208,42 +1208,42 @@
       <c r="B9" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="1"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="67" t="s">
+      <c r="L9" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="62" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="1"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
@@ -1254,19 +1254,19 @@
       <c r="B11" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="1"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
@@ -1277,19 +1277,19 @@
       <c r="B12" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="1"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="72" t="s">
+      <c r="L12" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
@@ -1300,27 +1300,27 @@
       <c r="B13" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
       <c r="H13" s="1"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="72" t="s">
+      <c r="L13" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
@@ -1331,9 +1331,9 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
       <c r="H15" s="26"/>
       <c r="J15" s="26"/>
     </row>
@@ -1341,18 +1341,18 @@
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
@@ -1363,9 +1363,9 @@
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
@@ -1385,20 +1385,20 @@
       <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="69" t="s">
+      <c r="L18" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1409,9 +1409,9 @@
       <c r="B19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
@@ -1431,9 +1431,9 @@
       <c r="B20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="59"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="58"/>
       <c r="L20" s="32"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
@@ -1445,9 +1445,9 @@
       <c r="B21" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="59"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
@@ -1464,9 +1464,9 @@
       <c r="B22" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="59"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="26"/>
@@ -1477,24 +1477,24 @@
       <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="59"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="L23" s="70" t="s">
+      <c r="L23" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="70"/>
-      <c r="N23" s="70"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
@@ -1503,9 +1503,9 @@
       <c r="B24" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="59"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="24"/>
       <c r="L24" s="36" t="s">
         <v>40</v>
@@ -1514,15 +1514,15 @@
       <c r="N24" s="36"/>
     </row>
     <row r="25" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="59"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="24"/>
       <c r="L25" s="36" t="s">
         <v>42</v>
@@ -1531,15 +1531,15 @@
       <c r="N25" s="36"/>
     </row>
     <row r="26" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="63" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="59"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="24"/>
       <c r="L26" s="36" t="s">
         <v>43</v>
@@ -1554,9 +1554,9 @@
       <c r="B27" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="24"/>
       <c r="L27" s="36" t="s">
         <v>45</v>
@@ -1565,15 +1565,15 @@
       <c r="N27" s="36"/>
     </row>
     <row r="28" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="63" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="L28" s="36" t="s">
@@ -1589,9 +1589,9 @@
       <c r="B29" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
       <c r="G29" s="24"/>
       <c r="L29" s="36" t="s">
         <v>48</v>
@@ -1604,16 +1604,16 @@
       <c r="B30" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="L30" s="67" t="s">
+      <c r="L30" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="67"/>
-      <c r="N30" s="67"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -1622,9 +1622,9 @@
       <c r="B31" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="55"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
       <c r="G31" s="38"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
@@ -1639,13 +1639,13 @@
       <c r="B32" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
       <c r="L32" s="36" t="s">
         <v>50</v>
       </c>
@@ -1657,22 +1657,22 @@
       <c r="B33" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="52"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
       <c r="L33" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
@@ -1686,9 +1686,9 @@
       <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
@@ -1699,15 +1699,15 @@
       <c r="P35" s="13"/>
     </row>
     <row r="36" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="73" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
@@ -1727,9 +1727,9 @@
       <c r="B37" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="49"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="54"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="53"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="26"/>
@@ -1749,9 +1749,9 @@
       <c r="B38" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="K38" s="25"/>
@@ -1763,9 +1763,9 @@
     </row>
     <row r="39" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
       <c r="K39" s="25"/>
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
@@ -1774,9 +1774,9 @@
       <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
@@ -1793,9 +1793,9 @@
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
@@ -1815,11 +1815,11 @@
       <c r="B42" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="53"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="45"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
@@ -1837,9 +1837,9 @@
       <c r="B43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -1853,9 +1853,9 @@
     <row r="44" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
@@ -1869,9 +1869,9 @@
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
       <c r="H45" s="26"/>
       <c r="J45" s="26"/>
       <c r="L45" s="12"/>
@@ -1886,9 +1886,9 @@
       <c r="B46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="54"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="53"/>
       <c r="F46" s="1"/>
       <c r="G46" s="26"/>
       <c r="H46" s="26"/>
@@ -1903,9 +1903,9 @@
     </row>
     <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
@@ -1916,78 +1916,78 @@
       <c r="N47" s="12"/>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="1:16" s="57" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="56"/>
-    </row>
-    <row r="49" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="48"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="55"/>
+    </row>
+    <row r="49" spans="1:15" s="56" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="L49" s="58" t="s">
+      <c r="L49" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="56"/>
-    </row>
-    <row r="50" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="55"/>
+    </row>
+    <row r="50" spans="1:15" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="L50" s="58" t="s">
+      <c r="L50" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="56"/>
-    </row>
-    <row r="51" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M50" s="57"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="55"/>
+    </row>
+    <row r="51" spans="1:15" s="56" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="56"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="55"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="17"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
       <c r="H52" s="26"/>
       <c r="J52" s="26"/>
       <c r="K52" s="17"/>
@@ -2003,9 +2003,9 @@
       <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -2142,7 +2142,7 @@
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="62" t="s">
+      <c r="A63" s="61" t="s">
         <v>81</v>
       </c>
       <c r="C63" s="26"/>
@@ -2156,7 +2156,7 @@
       <c r="O63" s="22"/>
     </row>
     <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="64" t="s">
+      <c r="A64" s="62" t="s">
         <v>82</v>
       </c>
       <c r="B64"/>

</xml_diff>

<commit_message>
Loader progress (you can now load trees, but not get rid of them somehow)
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEF7A41-F3FB-4EFD-B7AC-338C985FDEE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1AB34E-1C69-4F7D-9F56-D8C8CA610259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="396" windowWidth="30936" windowHeight="16416" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Description</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>René and Ivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                  </t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -546,6 +549,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -630,9 +646,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="7" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -642,7 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="11" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -673,9 +685,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -698,6 +707,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1025,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,67 +1097,67 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="66" t="s">
+      <c r="L1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-    </row>
-    <row r="3" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+    <row r="2" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+    </row>
+    <row r="3" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-    </row>
-    <row r="4" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+    </row>
+    <row r="4" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O5" s="2"/>
@@ -1149,10 +1167,10 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="26"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
       <c r="G6" s="26"/>
       <c r="I6" s="26"/>
       <c r="O6" s="13"/>
@@ -1165,19 +1183,19 @@
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="26"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
@@ -1188,19 +1206,19 @@
       <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="26"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="71" t="s">
+      <c r="L8" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1208,45 +1226,45 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="67" t="s">
+      <c r="L9" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
@@ -1254,22 +1272,22 @@
       <c r="A11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="26"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
       <c r="G11" s="26"/>
       <c r="H11" s="1"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="72" t="s">
+      <c r="L11" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
@@ -1277,22 +1295,22 @@
       <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="26"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="72" t="s">
+      <c r="L12" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
@@ -1300,31 +1318,31 @@
       <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="26"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
       <c r="G13" s="26"/>
       <c r="H13" s="1"/>
       <c r="I13" s="26"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="72" t="s">
+      <c r="L13" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="70"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="26"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
@@ -1334,9 +1352,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
       <c r="H15" s="26"/>
       <c r="J15" s="26"/>
     </row>
@@ -1344,18 +1363,18 @@
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="26"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
@@ -1366,10 +1385,10 @@
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="26"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="51"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -1388,20 +1407,20 @@
       <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="1"/>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="69" t="s">
+      <c r="L18" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1409,16 +1428,16 @@
       <c r="A19" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="26"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="26"/>
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
@@ -1431,12 +1450,13 @@
       <c r="A20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="59"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="53"/>
       <c r="L20" s="32"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
@@ -1445,13 +1465,13 @@
       <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="16"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="53"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
@@ -1464,13 +1484,13 @@
       <c r="A22" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="16"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="53"/>
       <c r="G22" s="16"/>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -1480,36 +1500,36 @@
       <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="24"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
       <c r="G23" s="24"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="L23" s="70" t="s">
+      <c r="L23" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="70"/>
-      <c r="N23" s="70"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="24"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
       <c r="L24" s="36" t="s">
         <v>40</v>
       </c>
@@ -1517,16 +1537,16 @@
       <c r="N24" s="36"/>
     </row>
     <row r="25" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="24"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
       <c r="L25" s="36" t="s">
         <v>42</v>
       </c>
@@ -1534,16 +1554,16 @@
       <c r="N25" s="36"/>
     </row>
     <row r="26" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="24"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
       <c r="L26" s="36" t="s">
         <v>43</v>
       </c>
@@ -1554,13 +1574,14 @@
       <c r="A27" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="24"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="72"/>
       <c r="L27" s="36" t="s">
         <v>45</v>
       </c>
@@ -1568,16 +1589,16 @@
       <c r="N27" s="36"/>
     </row>
     <row r="28" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="24"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="57"/>
       <c r="G28" s="24"/>
       <c r="L28" s="36" t="s">
         <v>47</v>
@@ -1589,13 +1610,15 @@
       <c r="A29" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
       <c r="G29" s="24"/>
+      <c r="H29" s="72"/>
       <c r="L29" s="36" t="s">
         <v>48</v>
       </c>
@@ -1604,31 +1627,33 @@
       <c r="A30" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
-      <c r="L30" s="67" t="s">
+      <c r="L30" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="67"/>
-      <c r="N30" s="67"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="55"/>
-      <c r="G31" s="38"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="71"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
       <c r="L31" s="36" t="s">
@@ -1639,16 +1664,16 @@
       <c r="A32" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
       <c r="L32" s="36" t="s">
         <v>50</v>
       </c>
@@ -1657,26 +1682,26 @@
       <c r="A33" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="52"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
       <c r="L33" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="26"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -1689,10 +1714,10 @@
       <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="26"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -1702,16 +1727,16 @@
       <c r="P35" s="13"/>
     </row>
     <row r="36" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="73" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="26"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="51"/>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -1727,13 +1752,13 @@
       <c r="A37" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="49"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="1"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
       <c r="G37" s="1"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -1749,12 +1774,13 @@
       <c r="A38" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="K38" s="25"/>
@@ -1766,9 +1792,10 @@
     </row>
     <row r="39" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
       <c r="K39" s="25"/>
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
@@ -1777,10 +1804,10 @@
       <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="26"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
       <c r="G40" s="26"/>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>
@@ -1796,10 +1823,10 @@
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="26"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="51"/>
       <c r="G41" s="26"/>
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
@@ -1815,14 +1842,14 @@
       <c r="A42" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="45"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="11"/>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
@@ -1840,10 +1867,10 @@
       <c r="B43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="1"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="J43" s="26"/>
@@ -1856,10 +1883,10 @@
     <row r="44" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="26"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
       <c r="G44" s="26"/>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
@@ -1872,9 +1899,10 @@
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
       <c r="H45" s="26"/>
       <c r="J45" s="26"/>
       <c r="L45" s="12"/>
@@ -1889,11 +1917,11 @@
       <c r="B46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="26"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="11"/>
       <c r="H46" s="26"/>
       <c r="I46" s="26"/>
       <c r="J46" s="26"/>
@@ -1906,10 +1934,10 @@
     </row>
     <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="26"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
       <c r="G47" s="26"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
@@ -1919,78 +1947,81 @@
       <c r="N47" s="12"/>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="1:16" s="57" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" s="55" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="56"/>
-    </row>
-    <row r="49" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="47"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="54"/>
+    </row>
+    <row r="49" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="1"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="52"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="L49" s="58" t="s">
+      <c r="L49" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="56"/>
-    </row>
-    <row r="50" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="54"/>
+    </row>
+    <row r="50" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="1"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="52"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="L50" s="58" t="s">
+      <c r="L50" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="56"/>
-    </row>
-    <row r="51" spans="1:15" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="54"/>
+    </row>
+    <row r="51" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="56"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="54"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="17"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
       <c r="H52" s="26"/>
       <c r="J52" s="26"/>
       <c r="K52" s="17"/>
@@ -2006,9 +2037,10 @@
       <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -2021,7 +2053,9 @@
       <c r="O53" s="2"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A54" s="29"/>
+      <c r="A54" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="C54" s="26"/>
       <c r="D54" s="26"/>
       <c r="H54" s="26"/>
@@ -2033,12 +2067,12 @@
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="29"/>
       <c r="C55" s="26"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
       <c r="J55" s="26"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
@@ -2128,7 +2162,7 @@
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="38" t="s">
         <v>70</v>
       </c>
       <c r="C62" s="26"/>
@@ -2145,7 +2179,7 @@
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="62" t="s">
+      <c r="A63" s="60" t="s">
         <v>81</v>
       </c>
       <c r="C63" s="26"/>
@@ -2159,7 +2193,7 @@
       <c r="O63" s="22"/>
     </row>
     <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="64" t="s">
+      <c r="A64" s="61" t="s">
         <v>82</v>
       </c>
       <c r="B64"/>

</xml_diff>

<commit_message>
Cleaned up old files
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA541BB-DF89-41C2-9B49-1F44667A6954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CEC4EA-EE77-43A7-B5DC-41BCD7B6AB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="396" windowWidth="30936" windowHeight="16416" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1981,7 +1981,7 @@
       <c r="O48" s="53"/>
     </row>
     <row r="49" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="54" t="s">

</xml_diff>

<commit_message>
planning update (just markings)
</commit_message>
<xml_diff>
--- a/Organization/Planning.xlsx
+++ b/Organization/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CEC4EA-EE77-43A7-B5DC-41BCD7B6AB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CDA5C8-C95D-4E00-BCA6-5736F06C78BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="396" windowWidth="30936" windowHeight="16416" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -626,9 +626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -642,9 +639,6 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="7"/>
@@ -659,7 +653,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="11" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -687,9 +680,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -719,6 +709,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,67 +1100,67 @@
         <v>44006</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-    </row>
-    <row r="3" spans="1:16" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="67" t="s">
+    <row r="2" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+    </row>
+    <row r="3" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-    </row>
-    <row r="4" spans="1:16" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+    </row>
+    <row r="4" spans="1:16" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="63"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="O5" s="2"/>
@@ -1170,13 +1170,13 @@
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="26"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
@@ -1187,42 +1187,42 @@
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="26"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="26"/>
-      <c r="L7" s="72" t="s">
+      <c r="L7" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
     <row r="8" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="1"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="26"/>
-      <c r="L8" s="72" t="s">
+      <c r="L8" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
@@ -1230,22 +1230,22 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="26"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="26"/>
-      <c r="L9" s="68" t="s">
+      <c r="L9" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
       <c r="O9" s="25"/>
       <c r="P9" s="13"/>
     </row>
@@ -1253,133 +1253,134 @@
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="26"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="26"/>
-      <c r="L10" s="68" t="s">
+      <c r="L10" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="26"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="26"/>
-      <c r="L11" s="73" t="s">
+      <c r="L11" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
     <row r="12" spans="1:16" s="14" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="26"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="26"/>
-      <c r="L12" s="73" t="s">
+      <c r="L12" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
     <row r="13" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="26"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="26"/>
-      <c r="L13" s="73" t="s">
+      <c r="L13" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="70"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="26"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="26"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="26"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="26"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
@@ -1390,13 +1391,13 @@
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="26"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="26"/>
       <c r="K17" s="8"/>
       <c r="L17" s="9" t="s">
@@ -1406,26 +1407,26 @@
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="26"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="26"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="70" t="s">
+      <c r="L18" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
@@ -1433,16 +1434,16 @@
       <c r="A19" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="1"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="26"/>
       <c r="K19" s="13"/>
       <c r="L19" s="12"/>
@@ -1455,223 +1456,231 @@
       <c r="A20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-    </row>
-    <row r="21" spans="1:16" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="45"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+    </row>
+    <row r="21" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="16"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
       <c r="J21" s="16"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
     </row>
     <row r="22" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="26"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
       <c r="J22" s="16"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="1"/>
-      <c r="L23" s="71" t="s">
+      <c r="C23" s="46"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="L23" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="71"/>
-      <c r="N23" s="71"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
     </row>
     <row r="24" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="L24" s="35" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="L24" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
     </row>
     <row r="25" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="L25" s="35" t="s">
+      <c r="C25" s="46"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="L25" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
     </row>
     <row r="26" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="L26" s="35" t="s">
+      <c r="C26" s="46"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="49"/>
+      <c r="L26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
     </row>
     <row r="27" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="L27" s="35" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="49"/>
+      <c r="L27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
     </row>
     <row r="28" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="65"/>
-      <c r="L28" s="35" t="s">
+      <c r="C28" s="46"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="49"/>
+      <c r="L28" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
     </row>
     <row r="29" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="65"/>
-      <c r="L29" s="35" t="s">
+      <c r="C29" s="46"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="49"/>
+      <c r="L29" s="34" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="16" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="L30" s="68" t="s">
+      <c r="C30" s="46"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="49"/>
+      <c r="L30" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
     </row>
     <row r="31" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="24"/>
-      <c r="L31" s="35" t="s">
+      <c r="C31" s="46"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="L31" s="34" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1679,17 +1688,17 @@
       <c r="A32" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="45"/>
-      <c r="L32" s="35" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="L32" s="34" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1697,29 +1706,29 @@
       <c r="A33" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="45"/>
-      <c r="L33" s="35" t="s">
+      <c r="C33" s="46"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="L33" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="26"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="26"/>
       <c r="K34" s="13"/>
       <c r="O34" s="13"/>
@@ -1729,77 +1738,78 @@
       <c r="A35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="26"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
       <c r="J35" s="26"/>
       <c r="K35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
     </row>
     <row r="36" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="59" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="26"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
       <c r="J36" s="26"/>
       <c r="K36" s="13"/>
-      <c r="L36" s="35" t="s">
+      <c r="L36" s="34" t="s">
         <v>65</v>
       </c>
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
     </row>
     <row r="37" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="26"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
       <c r="J37" s="26"/>
       <c r="K37" s="13"/>
-      <c r="L37" s="35" t="s">
+      <c r="L37" s="34" t="s">
         <v>66</v>
       </c>
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
     </row>
     <row r="38" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="47"/>
       <c r="K38" s="25"/>
-      <c r="L38" s="35" t="s">
+      <c r="L38" s="34" t="s">
         <v>67</v>
       </c>
       <c r="O38" s="25"/>
@@ -1807,12 +1817,13 @@
     </row>
     <row r="39" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
       <c r="K39" s="25"/>
       <c r="O39" s="25"/>
       <c r="P39" s="25"/>
@@ -1821,13 +1832,13 @@
       <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="26"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
       <c r="J40" s="26"/>
       <c r="K40" s="13"/>
       <c r="O40" s="13"/>
@@ -1840,13 +1851,13 @@
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="26"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
       <c r="J41" s="26"/>
       <c r="K41" s="13"/>
       <c r="L41" s="14" t="s">
@@ -1859,16 +1870,16 @@
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="26"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
       <c r="J42" s="26"/>
       <c r="K42" s="13"/>
       <c r="L42" s="14" t="s">
@@ -1878,18 +1889,19 @@
       <c r="P42" s="13"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="46"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="51"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="47"/>
       <c r="J43" s="26"/>
       <c r="L43" s="12" t="s">
         <v>62</v>
@@ -1900,13 +1912,13 @@
     <row r="44" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="9"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="26"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
       <c r="J44" s="26"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
@@ -1916,12 +1928,13 @@
       <c r="A45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
       <c r="J45" s="26"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
@@ -1935,13 +1948,13 @@
       <c r="B46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="26"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
       <c r="J46" s="26"/>
       <c r="L46" s="12" t="s">
         <v>61</v>
@@ -1952,100 +1965,103 @@
     </row>
     <row r="47" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="26"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
       <c r="J47" s="26"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
       <c r="O47" s="13"/>
     </row>
-    <row r="48" spans="1:16" s="54" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" s="51" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="53"/>
-    </row>
-    <row r="49" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="43"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="50"/>
+    </row>
+    <row r="49" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="1"/>
-      <c r="L49" s="55" t="s">
+      <c r="C49" s="43"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="L49" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="M49" s="55"/>
-      <c r="N49" s="55"/>
-      <c r="O49" s="53"/>
-    </row>
-    <row r="50" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="50"/>
+    </row>
+    <row r="50" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="46"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="1"/>
-      <c r="L50" s="55" t="s">
+      <c r="C50" s="43"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="L50" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="M50" s="55"/>
-      <c r="N50" s="55"/>
-      <c r="O50" s="53"/>
-    </row>
-    <row r="51" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+      <c r="O50" s="50"/>
+    </row>
+    <row r="51" spans="1:15" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="28"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="L51" s="55"/>
-      <c r="M51" s="55"/>
-      <c r="N51" s="55"/>
-      <c r="O51" s="53"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="50"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="17"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="47"/>
       <c r="J52" s="26"/>
       <c r="K52" s="17"/>
       <c r="L52" s="18"/>
@@ -2054,19 +2070,19 @@
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="46"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="51"/>
-      <c r="I53" s="1"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
       <c r="J53" s="26"/>
       <c r="L53" s="14" t="s">
         <v>60</v>
@@ -2090,12 +2106,12 @@
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="28"/>
       <c r="C55" s="26"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="38"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
       <c r="J55" s="26"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
@@ -2185,7 +2201,7 @@
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C62" s="26"/>
@@ -2202,7 +2218,7 @@
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="59" t="s">
+      <c r="A63" s="56" t="s">
         <v>81</v>
       </c>
       <c r="C63" s="26"/>
@@ -2216,7 +2232,7 @@
       <c r="O63" s="22"/>
     </row>
     <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="57" t="s">
         <v>82</v>
       </c>
       <c r="B64"/>

</xml_diff>